<commit_message>
Updated with few more MST tables
</commit_message>
<xml_diff>
--- a/Dokter_RDBMS.xlsx
+++ b/Dokter_RDBMS.xlsx
@@ -21,7 +21,7 @@
     <author>HP</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0">
+    <comment ref="D4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -37,7 +37,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0">
+    <comment ref="E4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -55,12 +55,43 @@
         </r>
       </text>
     </comment>
+    <comment ref="G4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Doctor
+Receptionist
+Accountant</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dentist
+Cardiologist
+Orthopaedic
+Neurologist</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>TBL_Group_MST</t>
   </si>
@@ -132,6 +163,36 @@
   </si>
   <si>
     <t>User_ID</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>TBL_Configuration_MST</t>
+  </si>
+  <si>
+    <t>TBL_User_Type_MST</t>
+  </si>
+  <si>
+    <t>UserType</t>
+  </si>
+  <si>
+    <t>TBL_Doctor_Specilization_MST</t>
+  </si>
+  <si>
+    <t>Specialization</t>
+  </si>
+  <si>
+    <t>TBL_Doctor_Spl_DTL</t>
+  </si>
+  <si>
+    <t>TBL_Feature_MST</t>
+  </si>
+  <si>
+    <t>FeatureName</t>
+  </si>
+  <si>
+    <t>Spelization_ID</t>
   </si>
 </sst>
 </file>
@@ -485,7 +546,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E9"/>
+  <dimension ref="A2:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -493,35 +554,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="21.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -534,71 +609,103 @@
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D7" s="1" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D8" s="1" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E9" s="1" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -610,20 +717,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -633,8 +740,11 @@
       <c r="C2" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -644,8 +754,11 @@
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -654,6 +767,9 @@
       </c>
       <c r="C4" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>